<commit_message>
Added script to simulate average power use per hour
</commit_message>
<xml_diff>
--- a/data/AESO Hourly Power Load Averaged.xlsx
+++ b/data/AESO Hourly Power Load Averaged.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cd3e99d6a3c3959/Documents/2018 UBC/MECH 431/MECH431/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moochster\OneDrive\Documents\2018 UBC\MECH 431\MECH431\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{136F2FC7-2F9E-4E42-B3AC-9D19CC69E0BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{136F2FC7-2F9E-4E42-B3AC-9D19CC69E0BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D13D0E0C-23DD-4601-BEE3-67190D993617}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="18225" windowHeight="8595"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="18225" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AESO Hourly Power Load Averaged" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3474,11 +3474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>